<commit_message>
forgot to safe. Ready for keying dimensions
</commit_message>
<xml_diff>
--- a/calculations/MIL-DTL-38999-III_dimension_table.xlsx
+++ b/calculations/MIL-DTL-38999-III_dimension_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lelem\git_repositories\projects\D38999-3MF\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20541C78-62AC-4E01-8DAB-75A94C515F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F18341-0C02-46EF-B3E1-2C07624A807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{58E9E39D-3151-410B-8DC1-39983DB63DF0}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>